<commit_message>
updates to outputs and rmd files for chapters 1,2 and 3. Updated figures to follow and final chpater 2 to follow
</commit_message>
<xml_diff>
--- a/tables/chapter_2/table_1.xlsx
+++ b/tables/chapter_2/table_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>Morphological Characteristic</t>
   </si>
@@ -30,15 +30,9 @@
     <t>Grams (g)</t>
   </si>
   <si>
-    <t>Primary length</t>
-  </si>
-  <si>
     <t>Millimeters (mm)</t>
   </si>
   <si>
-    <t>Primary width</t>
-  </si>
-  <si>
     <t>Frond length</t>
   </si>
   <si>
@@ -61,13 +55,43 @@
   </si>
   <si>
     <t>Total length</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Ecklonia maxima</t>
+  </si>
+  <si>
+    <t>Laminaria pallida</t>
+  </si>
+  <si>
+    <t>Stipe diameter</t>
+  </si>
+  <si>
+    <t>Number of digits</t>
+  </si>
+  <si>
+    <t>Primary blade length</t>
+  </si>
+  <si>
+    <t>Primary blade width</t>
+  </si>
+  <si>
+    <t>Lamina blade weight</t>
+  </si>
+  <si>
+    <t>Lamina blade length</t>
+  </si>
+  <si>
+    <t>Lamina blade thickness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +112,14 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -103,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -112,54 +144,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -167,20 +162,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,104 +474,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated raw table files and delted unneeded
</commit_message>
<xml_diff>
--- a/tables/chapter_2/table_1.xlsx
+++ b/tables/chapter_2/table_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>Morphological Characteristic</t>
   </si>
@@ -72,19 +72,28 @@
     <t>Number of digits</t>
   </si>
   <si>
-    <t>Primary blade length</t>
-  </si>
-  <si>
-    <t>Primary blade width</t>
-  </si>
-  <si>
-    <t>Lamina blade weight</t>
-  </si>
-  <si>
-    <t>Lamina blade length</t>
-  </si>
-  <si>
-    <t>Lamina blade thickness</t>
+    <t>Kilograms (kg)</t>
+  </si>
+  <si>
+    <t>Centimeters (cm)</t>
+  </si>
+  <si>
+    <t>Lamina weight</t>
+  </si>
+  <si>
+    <t>Lamina length</t>
+  </si>
+  <si>
+    <t>Lamina thickness</t>
+  </si>
+  <si>
+    <t>Primary length</t>
+  </si>
+  <si>
+    <t>Primary width</t>
+  </si>
+  <si>
+    <t>Thallus mass</t>
   </si>
 </sst>
 </file>
@@ -474,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,10 +523,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,10 +534,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -539,7 +548,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -550,7 +559,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -561,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -594,7 +603,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -605,7 +614,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,7 +625,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,8 +635,8 @@
       <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>4</v>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -648,8 +657,8 @@
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>3</v>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,8 +668,8 @@
       <c r="B16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>4</v>
+      <c r="C16" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -683,6 +692,28 @@
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>